<commit_message>
fix/Pit stops timing and data mining
</commit_message>
<xml_diff>
--- a/Docs/LalaLaunch_Backlog.xlsx
+++ b/Docs/LalaLaunch_Backlog.xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy_\Documents\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A45EC-69F6-4196-853A-CF20874A959E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E37157-35FB-4E1A-8C36-E9724237D942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Glossary" sheetId="2" r:id="rId2"/>
-    <sheet name="HowTo" sheetId="3" r:id="rId3"/>
-    <sheet name="Ideas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -106,6 +103,36 @@
     <t>LALA-016</t>
   </si>
   <si>
+    <t>LALA-017</t>
+  </si>
+  <si>
+    <t>LALA-018</t>
+  </si>
+  <si>
+    <t>LALA-019</t>
+  </si>
+  <si>
+    <t>LALA-020</t>
+  </si>
+  <si>
+    <t>LALA-021</t>
+  </si>
+  <si>
+    <t>LALA-022</t>
+  </si>
+  <si>
+    <t>LALA-023</t>
+  </si>
+  <si>
+    <t>LALA-024</t>
+  </si>
+  <si>
+    <t>LALA-025</t>
+  </si>
+  <si>
+    <t>LALA-026</t>
+  </si>
+  <si>
     <t>P0</t>
   </si>
   <si>
@@ -160,6 +187,27 @@
     <t>UX</t>
   </si>
   <si>
+    <t>Telemetry / API</t>
+  </si>
+  <si>
+    <t>Naming / API</t>
+  </si>
+  <si>
+    <t>Profiles / UX</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Docs</t>
+  </si>
+  <si>
+    <t>UI / Dash</t>
+  </si>
+  <si>
     <t>Pre-grid fuel warning (one-stint)</t>
   </si>
   <si>
@@ -208,6 +256,36 @@
     <t>Driver vs Engineer mode toggle</t>
   </si>
   <si>
+    <t>Expose pit phase (Pit.Phase)</t>
+  </si>
+  <si>
+    <t>Standardise new SimHub property names (drop extra 'Lala.')</t>
+  </si>
+  <si>
+    <t>DTL auto‑fill and candidate apply</t>
+  </si>
+  <si>
+    <t>Save hygiene tolerance for DTL</t>
+  </si>
+  <si>
+    <t>Mine tyre‑change delta</t>
+  </si>
+  <si>
+    <t>Mine refuel rate (L/s)</t>
+  </si>
+  <si>
+    <t>Expose Pit.FormulaTopSec (debug)</t>
+  </si>
+  <si>
+    <t>Wet/dry baseline selection</t>
+  </si>
+  <si>
+    <t>Property naming map in README</t>
+  </si>
+  <si>
+    <t>Service stop loss (DTL + Stop) property – document and demo</t>
+  </si>
+  <si>
     <t>Warn before rolling if current fuel cannot finish a no-stop race given profile avg fuel/lap, wet factor, contingency, race length.</t>
   </si>
   <si>
@@ -256,6 +334,36 @@
     <t>Toggle to hide/show advanced controls; driver sees target fuel, fuel-to-add, laps-to-box, PB.</t>
   </si>
   <si>
+    <t>Publish current pit cycle phase as idle, pit-lap, or out-lap for use on dashes and testing overlays.</t>
+  </si>
+  <si>
+    <t>For new properties use canonical names without the extra 'Lala.' segment. Keep existing names as aliases for backward compatibility and document the mapping.</t>
+  </si>
+  <si>
+    <t>If profile pit‑lane loss is empty/0, auto‑fill on first valid stop. Otherwise show 'New candidate: Xs' with an Apply button to commit. Provide a Reset button to default (configurable).</t>
+  </si>
+  <si>
+    <t>Avoid churn by only saving profile pit‑lane loss when |new − current| ≥ 0.5 s. Log whether save was suppressed or performed, and the source (direct/formula).</t>
+  </si>
+  <si>
+    <t>From stops with wheel changes, estimate tyre‑change time; maintain rolling median and sample count; surface as candidate with Apply button.</t>
+  </si>
+  <si>
+    <t>From fuel‑only stops, compute effective refuel rate; maintain rolling median; ignore mixed tyre+fuel stops that skew the rate; surface as candidate with Apply.</t>
+  </si>
+  <si>
+    <t>Publish (PitLap − Stop + OutLap) as a diagnostic to explain DTL changes across layouts and baselines.</t>
+  </si>
+  <si>
+    <t>When track condition is Wet, prefer profile wet average; otherwise prefer profile dry average; fallback chain remains as today.</t>
+  </si>
+  <si>
+    <t>Add a table that lists canonical property names and deprecated aliases so dashes can transition cleanly.</t>
+  </si>
+  <si>
+    <t>Document the Service stop loss property and include in the sample dash for strategy gap estimation.</t>
+  </si>
+  <si>
     <t>Shows deficit &gt; 0 L only in Race sessions; works for lap- or time-based races; exposes SimHub params Lala.Fuel.PreGrid.RequiredFuelL, DeficitL, LowFuel.</t>
   </si>
   <si>
@@ -304,6 +412,36 @@
     <t>Single toggle flips visibility groups; persists per user; no layout churn.</t>
   </si>
   <si>
+    <t>Property is present; shows 'pit-lap' at S/F after pit exit; shows 'out-lap' at S/F after pit box; returns 'idle' otherwise; validated on two replay stops.</t>
+  </si>
+  <si>
+    <t>New delegates exposed without 'Lala.'; existing dash bindings continue to work; README contains mapping table of old→new names.</t>
+  </si>
+  <si>
+    <t>1) Auto‑fill occurs only when current = 0; 2) Candidate banner appears after valid stop; 3) Apply updates profile and UI; 4) Reset restores default value.</t>
+  </si>
+  <si>
+    <t>Small deltas (&lt;0.5 s) do not write; log shows 'suppressed' vs 'saved' with timestamp and source.</t>
+  </si>
+  <si>
+    <t>Candidate value and sample count shown; Apply writes to profile; confidence displayed.</t>
+  </si>
+  <si>
+    <t>Candidate with sample count visible; Apply persists and it is used by pit‑time calculator.</t>
+  </si>
+  <si>
+    <t>Property equals arithmetic from log within ±0.01 s on two replay stops.</t>
+  </si>
+  <si>
+    <t>Source label shows 'profile‑avg‑wet' or 'profile‑avg'; numbers match profile values.</t>
+  </si>
+  <si>
+    <t>README contains mapping table and note on deprecation policy.</t>
+  </si>
+  <si>
+    <t>Property visible; sample dash updated; validated on replay stops.</t>
+  </si>
+  <si>
     <t>Backlog</t>
   </si>
   <si>
@@ -314,75 +452,6 @@
   </si>
   <si>
     <t>v0.5.0</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>P0 = next release scope; P1 = next wave.</t>
-  </si>
-  <si>
-    <t>Backlog, Todo, Doing, Done, Blocked.</t>
-  </si>
-  <si>
-    <t>Subsystem (Fuel, Profiles, Pit, Strategy, Rejoin, SimHub params, etc.).</t>
-  </si>
-  <si>
-    <t>Milestone label (e.g., v0.4.0).</t>
-  </si>
-  <si>
-    <t>Never persist temps/sample counts; track keys are canonical; display names are UI-only.</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Add to GitHub</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Editing</t>
-  </si>
-  <si>
-    <t>Linking</t>
-  </si>
-  <si>
-    <t>2025-09-15</t>
-  </si>
-  <si>
-    <t>Single source of truth for LalaLaunch backlog; upload to GitHub under planning/.</t>
-  </si>
-  <si>
-    <t>Repo → Add file → Upload files → create folder 'planning/' → upload this .xlsx → Commit to main.</t>
-  </si>
-  <si>
-    <t>Create a GitHub Project later and mirror items as Issues; Excel stays source of truth for now.</t>
-  </si>
-  <si>
-    <t>Add new rows at the bottom; keep IDs unique (LALA-###).</t>
-  </si>
-  <si>
-    <t>Paste Issue URL in 'GitHub Issue Link' once created.</t>
-  </si>
-  <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>Idea</t>
   </si>
 </sst>
 </file>
@@ -441,19 +510,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,27 +825,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="18.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="45" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="11.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="55.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,10 +859,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -814,62 +881,62 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>77</v>
+        <v>62</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -877,28 +944,28 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -906,28 +973,28 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -935,57 +1002,57 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>81</v>
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -993,86 +1060,86 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1080,28 +1147,28 @@
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1109,57 +1176,57 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1167,28 +1234,28 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1196,57 +1263,57 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1254,185 +1321,318 @@
         <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
+      <c r="F27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Most fixes done. Just immediate publish of data needed
</commit_message>
<xml_diff>
--- a/Docs/LalaLaunch_Backlog.xlsx
+++ b/Docs/LalaLaunch_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy_\Documents\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E37157-35FB-4E1A-8C36-E9724237D942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64AE5B-519E-4AAF-9727-888060EE09CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29205" yWindow="-3810" windowWidth="37230" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -452,6 +452,24 @@
   </si>
   <si>
     <t>v0.5.0</t>
+  </si>
+  <si>
+    <t>LALA-027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI  </t>
+  </si>
+  <si>
+    <t>Tire change time changing total fuel unecessarily</t>
+  </si>
+  <si>
+    <t>Changing tire time that is still less than refuel time is adjusting fuel when it shouldn't because the time is already accounted by the refuel time.</t>
+  </si>
+  <si>
+    <t>When tire change time is less than refuel time, the total fuel needed should not change</t>
+  </si>
+  <si>
+    <t>any</t>
   </si>
 </sst>
 </file>
@@ -825,10 +843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,8 +856,8 @@
     <col min="2" max="2" width="8.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="55.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="56.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="69.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="3" customWidth="1"/>
@@ -1635,6 +1654,35 @@
         <v>142</v>
       </c>
     </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix pit stop clean up (#13)
* initial draft fixes

* initial clean pre test

* Most fixes done. Just immediate publish of data needed
</commit_message>
<xml_diff>
--- a/Docs/LalaLaunch_Backlog.xlsx
+++ b/Docs/LalaLaunch_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy_\Documents\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E37157-35FB-4E1A-8C36-E9724237D942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64AE5B-519E-4AAF-9727-888060EE09CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29205" yWindow="-3810" windowWidth="37230" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -452,6 +452,24 @@
   </si>
   <si>
     <t>v0.5.0</t>
+  </si>
+  <si>
+    <t>LALA-027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI  </t>
+  </si>
+  <si>
+    <t>Tire change time changing total fuel unecessarily</t>
+  </si>
+  <si>
+    <t>Changing tire time that is still less than refuel time is adjusting fuel when it shouldn't because the time is already accounted by the refuel time.</t>
+  </si>
+  <si>
+    <t>When tire change time is less than refuel time, the total fuel needed should not change</t>
+  </si>
+  <si>
+    <t>any</t>
   </si>
 </sst>
 </file>
@@ -825,10 +843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,8 +856,8 @@
     <col min="2" max="2" width="8.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="55.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="56.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="69.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="3" customWidth="1"/>
@@ -1635,6 +1654,35 @@
         <v>142</v>
       </c>
     </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>